<commit_message>
20250917 running tests, code is solid
</commit_message>
<xml_diff>
--- a/combined_cal_data.xlsx
+++ b/combined_cal_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LINER\Documents\PycharmProjects\20250812_EVM_DPD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LINER\Documents\PycharmProjects\20250804_Power_Servo\src\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A20C102-DBE6-4CD6-A878-034E3F2C44D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946A4763-D5F1-4269-B29C-E57FBDBAF1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27888" yWindow="2148" windowWidth="27000" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Calibration" sheetId="1" r:id="rId1"/>
@@ -33,15 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Test Set_Input</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Center Frequency (GHz)</t>
-  </si>
-  <si>
-    <t>Set Power (dBm)_Input</t>
   </si>
   <si>
     <t>VSG Offset (dB)</t>
@@ -54,6 +48,9 @@
   </si>
   <si>
     <t>Output Power Offset (dB)</t>
+  </si>
+  <si>
+    <t>Test Set</t>
   </si>
 </sst>
 </file>
@@ -416,47 +413,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -464,22 +457,19 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>-1.4319999999999999</v>
       </c>
       <c r="D2">
-        <v>1.4419999999999999</v>
+        <v>15.819000000000001</v>
       </c>
       <c r="E2">
-        <v>18.877376299999998</v>
+        <v>1.5880000000000001</v>
       </c>
       <c r="F2">
-        <v>4.9106467590000005</v>
-      </c>
-      <c r="G2">
-        <v>13.286999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.186999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -487,22 +477,19 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>-1.46</v>
       </c>
       <c r="D3">
-        <v>1.4510000000000001</v>
+        <v>15.942</v>
       </c>
       <c r="E3">
-        <v>18.961090820000003</v>
+        <v>1.603</v>
       </c>
       <c r="F3">
-        <v>4.8543453521999993</v>
-      </c>
-      <c r="G3">
-        <v>13.364000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.311999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -510,22 +497,19 @@
         <v>2.1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-1.476</v>
       </c>
       <c r="D4">
-        <v>1.466</v>
+        <v>16.05</v>
       </c>
       <c r="E4">
-        <v>19.121470480000003</v>
+        <v>1.615</v>
       </c>
       <c r="F4">
-        <v>4.8970604094999999</v>
-      </c>
-      <c r="G4">
-        <v>13.628</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.519</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -533,22 +517,19 @@
         <v>2.15</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-1.468</v>
       </c>
       <c r="D5">
-        <v>1.4550000000000001</v>
+        <v>16.123999999999999</v>
       </c>
       <c r="E5">
-        <v>19.178368080000002</v>
+        <v>1.583</v>
       </c>
       <c r="F5">
-        <v>4.8937490692000001</v>
-      </c>
-      <c r="G5">
-        <v>13.847999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.755000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -556,22 +537,19 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>-1.488</v>
       </c>
       <c r="D6">
-        <v>1.4870000000000001</v>
+        <v>16.170000000000002</v>
       </c>
       <c r="E6">
-        <v>19.197285770999997</v>
+        <v>1.577</v>
       </c>
       <c r="F6">
-        <v>4.7988591460999999</v>
-      </c>
-      <c r="G6">
-        <v>14.100999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.042</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -579,22 +557,19 @@
         <v>2.25</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>-1.5089999999999999</v>
       </c>
       <c r="D7">
-        <v>1.516</v>
+        <v>16.170000000000002</v>
       </c>
       <c r="E7">
-        <v>19.283983999999997</v>
+        <v>1.58</v>
       </c>
       <c r="F7">
-        <v>4.8966070557000005</v>
-      </c>
-      <c r="G7">
-        <v>14.455</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -602,22 +577,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>-1.542</v>
       </c>
       <c r="D8">
-        <v>1.484</v>
+        <v>16.125</v>
       </c>
       <c r="E8">
-        <v>19.174363630000002</v>
+        <v>1.5289999999999999</v>
       </c>
       <c r="F8">
-        <v>4.8363657990000002</v>
-      </c>
-      <c r="G8">
-        <v>14.562000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -625,22 +597,19 @@
         <v>2.35</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>-1.5669999999999999</v>
       </c>
       <c r="D9">
-        <v>1.4710000000000001</v>
+        <v>16.055</v>
       </c>
       <c r="E9">
-        <v>19.056797876999997</v>
+        <v>1.605</v>
       </c>
       <c r="F9">
-        <v>4.8357852325000001</v>
-      </c>
-      <c r="G9">
-        <v>14.581</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.582000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -648,22 +617,19 @@
         <v>2.4</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>-1.5089999999999999</v>
       </c>
       <c r="D10">
-        <v>1.554</v>
+        <v>15.952</v>
       </c>
       <c r="E10">
-        <v>19.245097799999996</v>
+        <v>1.6160000000000001</v>
       </c>
       <c r="F10">
-        <v>5.1142127380000009</v>
-      </c>
-      <c r="G10">
-        <v>14.803000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.516</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -671,22 +637,19 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>-1.5669999999999999</v>
       </c>
       <c r="D11">
-        <v>1.5389999999999999</v>
+        <v>15.826000000000001</v>
       </c>
       <c r="E11">
-        <v>18.930910560000001</v>
+        <v>1.5820000000000001</v>
       </c>
       <c r="F11">
-        <v>5.0084304657000001</v>
-      </c>
-      <c r="G11">
-        <v>14.442</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.281000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -694,22 +657,19 @@
         <v>2.5</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>-1.5880000000000001</v>
       </c>
       <c r="D12">
-        <v>1.522</v>
+        <v>15.7</v>
       </c>
       <c r="E12">
-        <v>18.852705889999999</v>
+        <v>1.669</v>
       </c>
       <c r="F12">
-        <v>5.0801656494000005</v>
-      </c>
-      <c r="G12">
-        <v>14.249000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.09</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -717,22 +677,19 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>-1.58</v>
       </c>
       <c r="D13">
-        <v>1.528</v>
+        <v>15.579000000000001</v>
       </c>
       <c r="E13">
-        <v>18.8173262</v>
+        <v>1.6759999999999999</v>
       </c>
       <c r="F13">
-        <v>5.2027894287000009</v>
-      </c>
-      <c r="G13">
-        <v>14.08</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.792999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -740,22 +697,19 @@
         <v>2.6</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>-1.597</v>
       </c>
       <c r="D14">
-        <v>1.5660000000000001</v>
+        <v>15.467000000000001</v>
       </c>
       <c r="E14">
-        <v>18.752407669999997</v>
+        <v>1.6839999999999999</v>
       </c>
       <c r="F14">
-        <v>5.2723601073999999</v>
-      </c>
-      <c r="G14">
-        <v>13.879000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.523</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -763,22 +717,19 @@
         <v>2.65</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>-1.6259999999999999</v>
       </c>
       <c r="D15">
-        <v>1.5609999999999999</v>
+        <v>15.382999999999999</v>
       </c>
       <c r="E15">
-        <v>18.6745047</v>
+        <v>1.748</v>
       </c>
       <c r="F15">
-        <v>5.3430361022999993</v>
-      </c>
-      <c r="G15">
-        <v>13.683</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.372999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -786,22 +737,19 @@
         <v>2.7</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>-1.6339999999999999</v>
       </c>
       <c r="D16">
-        <v>1.569</v>
+        <v>15.326000000000001</v>
       </c>
       <c r="E16">
-        <v>18.6479672</v>
+        <v>1.7569999999999999</v>
       </c>
       <c r="F16">
-        <v>5.4496345367000005</v>
-      </c>
-      <c r="G16">
-        <v>13.653</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.257999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -809,22 +757,19 @@
         <v>2.75</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>-1.649</v>
       </c>
       <c r="D17">
-        <v>1.6120000000000001</v>
+        <v>15.297000000000001</v>
       </c>
       <c r="E17">
-        <v>18.634738810000002</v>
+        <v>1.7949999999999999</v>
       </c>
       <c r="F17">
-        <v>5.4528428345000002</v>
-      </c>
-      <c r="G17">
-        <v>13.685</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.271000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -832,22 +777,19 @@
         <v>2.8</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>-1.6930000000000001</v>
       </c>
       <c r="D18">
-        <v>1.621</v>
+        <v>15.305999999999999</v>
       </c>
       <c r="E18">
-        <v>18.69280895</v>
+        <v>1.8</v>
       </c>
       <c r="F18">
-        <v>4.968410476679999</v>
-      </c>
-      <c r="G18">
-        <v>13.803999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.359</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -855,22 +797,19 @@
         <v>2.85</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>-1.7230000000000001</v>
       </c>
       <c r="D19">
-        <v>1.601</v>
+        <v>15.345000000000001</v>
       </c>
       <c r="E19">
-        <v>18.790691399999996</v>
+        <v>1.7689999999999999</v>
       </c>
       <c r="F19">
-        <v>5.4923536529999994</v>
-      </c>
-      <c r="G19">
-        <v>14.018000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.502000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -878,22 +817,19 @@
         <v>2.9</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>-1.704</v>
       </c>
       <c r="D20">
-        <v>1.6359999999999999</v>
+        <v>15.414999999999999</v>
       </c>
       <c r="E20">
-        <v>18.71617741</v>
+        <v>1.784</v>
       </c>
       <c r="F20">
-        <v>5.3400157623000002</v>
-      </c>
-      <c r="G20">
-        <v>14.097</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.763</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -901,22 +837,19 @@
         <v>2.95</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>-1.6859999999999999</v>
       </c>
       <c r="D21">
-        <v>1.673</v>
+        <v>15.513999999999999</v>
       </c>
       <c r="E21">
-        <v>19.005667990000003</v>
+        <v>1.806</v>
       </c>
       <c r="F21">
-        <v>5.5386509857000004</v>
-      </c>
-      <c r="G21">
-        <v>14.577999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.071</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -924,22 +857,19 @@
         <v>3</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>-1.7310000000000001</v>
       </c>
       <c r="D22">
-        <v>1.635</v>
+        <v>15.627000000000001</v>
       </c>
       <c r="E22">
-        <v>19.065814580000001</v>
+        <v>1.7350000000000001</v>
       </c>
       <c r="F22">
-        <v>5.4870238036999996</v>
-      </c>
-      <c r="G22">
-        <v>14.776</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.282</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -947,22 +877,19 @@
         <v>3.05</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>-1.7929999999999999</v>
       </c>
       <c r="D23">
-        <v>1.7110000000000001</v>
+        <v>15.756</v>
       </c>
       <c r="E23">
-        <v>19.271046599999998</v>
+        <v>1.7949999999999999</v>
       </c>
       <c r="F23">
-        <v>5.6027765502999998</v>
-      </c>
-      <c r="G23">
-        <v>15.077999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.567</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -970,22 +897,19 @@
         <v>3.1</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>-1.8029999999999999</v>
       </c>
       <c r="D24">
-        <v>1.74</v>
+        <v>15.888</v>
       </c>
       <c r="E24">
-        <v>19.49373039</v>
+        <v>1.837</v>
       </c>
       <c r="F24">
-        <v>5.6259754791000001</v>
-      </c>
-      <c r="G24">
-        <v>15.288</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.724</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -993,22 +917,19 @@
         <v>3.15</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>-1.8129999999999999</v>
       </c>
       <c r="D25">
-        <v>1.7230000000000001</v>
+        <v>16.010000000000002</v>
       </c>
       <c r="E25">
-        <v>19.670087599999999</v>
+        <v>1.8380000000000001</v>
       </c>
       <c r="F25">
-        <v>5.6309813995000004</v>
-      </c>
-      <c r="G25">
-        <v>15.294</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.706</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1016,22 +937,19 @@
         <v>3.2</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>-1.83</v>
       </c>
       <c r="D26">
-        <v>1.738</v>
+        <v>16.109000000000002</v>
       </c>
       <c r="E26">
-        <v>19.746206150000003</v>
+        <v>1.85</v>
       </c>
       <c r="F26">
-        <v>5.7057594757000007</v>
-      </c>
-      <c r="G26">
-        <v>15.186</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.564</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1039,22 +957,19 @@
         <v>3.25</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>-1.8260000000000001</v>
       </c>
       <c r="D27">
-        <v>1.7509999999999999</v>
+        <v>16.183</v>
       </c>
       <c r="E27">
-        <v>19.890292500000001</v>
+        <v>1.87</v>
       </c>
       <c r="F27">
-        <v>5.8066486359000002</v>
-      </c>
-      <c r="G27">
-        <v>15.003</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.334</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1062,22 +977,19 @@
         <v>3.3</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>-1.8480000000000001</v>
       </c>
       <c r="D28">
-        <v>1.754</v>
+        <v>16.216000000000001</v>
       </c>
       <c r="E28">
-        <v>19.920258400000002</v>
+        <v>1.9039999999999999</v>
       </c>
       <c r="F28">
-        <v>5.7670138245000002</v>
-      </c>
-      <c r="G28">
-        <v>14.771000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.068</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1085,22 +997,19 @@
         <v>3.35</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>-1.8520000000000001</v>
       </c>
       <c r="D29">
-        <v>1.7809999999999999</v>
+        <v>16.209</v>
       </c>
       <c r="E29">
-        <v>19.941718499999997</v>
+        <v>1.9339999999999999</v>
       </c>
       <c r="F29">
-        <v>5.927026550299999</v>
-      </c>
-      <c r="G29">
-        <v>14.550999999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.801</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1108,22 +1017,19 @@
         <v>3.4</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>-1.867</v>
       </c>
       <c r="D30">
-        <v>1.76</v>
+        <v>16.170000000000002</v>
       </c>
       <c r="E30">
-        <v>19.947668700000001</v>
+        <v>1.966</v>
       </c>
       <c r="F30">
-        <v>5.9823266295999993</v>
-      </c>
-      <c r="G30">
-        <v>14.390999999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1131,22 +1037,19 @@
         <v>3.45</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>-1.8680000000000001</v>
       </c>
       <c r="D31">
-        <v>1.8009999999999999</v>
+        <v>16.091999999999999</v>
       </c>
       <c r="E31">
-        <v>19.870635700000001</v>
+        <v>1.978</v>
       </c>
       <c r="F31">
-        <v>6.0741763306000003</v>
-      </c>
-      <c r="G31">
-        <v>14.34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.442</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1154,22 +1057,19 @@
         <v>3.5</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>-1.9059999999999999</v>
       </c>
       <c r="D32">
-        <v>1.804</v>
+        <v>15.987</v>
       </c>
       <c r="E32">
-        <v>19.8170477</v>
+        <v>2.012</v>
       </c>
       <c r="F32">
-        <v>6.1367076569000005</v>
-      </c>
-      <c r="G32">
-        <v>14.261000000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.411</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1177,22 +1077,19 @@
         <v>3.55</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>-1.9179999999999999</v>
       </c>
       <c r="D33">
-        <v>1.8069999999999999</v>
+        <v>15.872</v>
       </c>
       <c r="E33">
-        <v>19.7635553</v>
+        <v>2.04</v>
       </c>
       <c r="F33">
-        <v>6.1751378784000002</v>
-      </c>
-      <c r="G33">
-        <v>14.346</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.468</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1200,22 +1097,19 @@
         <v>3.6</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>-1.923</v>
       </c>
       <c r="D34">
-        <v>1.851</v>
+        <v>15.749000000000001</v>
       </c>
       <c r="E34">
-        <v>19.719733099999999</v>
+        <v>2.008</v>
       </c>
       <c r="F34">
-        <v>6.1977502136000009</v>
-      </c>
-      <c r="G34">
-        <v>14.546999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.561</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1223,22 +1117,19 @@
         <v>3.65</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>-1.966</v>
       </c>
       <c r="D35">
-        <v>1.8520000000000001</v>
+        <v>15.634</v>
       </c>
       <c r="E35">
-        <v>19.560719799999998</v>
+        <v>2.02</v>
       </c>
       <c r="F35">
-        <v>6.1280187836000009</v>
-      </c>
-      <c r="G35">
-        <v>14.691000000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.781000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1246,22 +1137,19 @@
         <v>3.7</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>-1.96</v>
       </c>
       <c r="D36">
-        <v>1.86</v>
+        <v>15.532</v>
       </c>
       <c r="E36">
-        <v>19.480172200000002</v>
+        <v>2.0310000000000001</v>
       </c>
       <c r="F36">
-        <v>6.1683208617999998</v>
-      </c>
-      <c r="G36">
-        <v>14.957999999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.047000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1269,22 +1157,19 @@
         <v>3.75</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>-1.972</v>
       </c>
       <c r="D37">
-        <v>1.8839999999999999</v>
+        <v>15.46</v>
       </c>
       <c r="E37">
-        <v>19.412072800000001</v>
+        <v>1.986</v>
       </c>
       <c r="F37">
-        <v>6.2180649261000003</v>
-      </c>
-      <c r="G37">
-        <v>15.222</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.278</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1292,22 +1177,19 @@
         <v>3.8</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>-1.9970000000000001</v>
       </c>
       <c r="D38">
-        <v>1.89</v>
+        <v>15.414</v>
       </c>
       <c r="E38">
-        <v>19.3710135</v>
+        <v>2.0030000000000001</v>
       </c>
       <c r="F38">
-        <v>6.2334114837999994</v>
-      </c>
-      <c r="G38">
-        <v>15.456</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1315,22 +1197,19 @@
         <v>3.85</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>-2.0310000000000001</v>
       </c>
       <c r="D39">
-        <v>1.9019999999999999</v>
+        <v>15.393000000000001</v>
       </c>
       <c r="E39">
-        <v>19.335982200000004</v>
+        <v>1.992</v>
       </c>
       <c r="F39">
-        <v>6.1906648864999996</v>
-      </c>
-      <c r="G39">
-        <v>15.608999999999998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.672000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1338,22 +1217,19 @@
         <v>3.9</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>-2.0329999999999999</v>
       </c>
       <c r="D40">
-        <v>1.9470000000000001</v>
+        <v>15.407999999999999</v>
       </c>
       <c r="E40">
-        <v>19.446208680000002</v>
+        <v>1.992</v>
       </c>
       <c r="F40">
-        <v>5.7463212280000002</v>
-      </c>
-      <c r="G40">
-        <v>15.725999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.712</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1361,22 +1237,19 @@
         <v>3.95</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>-2.0310000000000001</v>
       </c>
       <c r="D41">
-        <v>1.9630000000000001</v>
+        <v>15.451000000000001</v>
       </c>
       <c r="E41">
-        <v>19.522127810000001</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="F41">
-        <v>6.3046727600000008</v>
-      </c>
-      <c r="G41">
-        <v>15.694000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.635</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1384,22 +1257,19 @@
         <v>4</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>-2.0579999999999998</v>
       </c>
       <c r="D42">
-        <v>1.929</v>
+        <v>15.521000000000001</v>
       </c>
       <c r="E42">
-        <v>19.555593799999997</v>
+        <v>2.0579999999999998</v>
       </c>
       <c r="F42">
-        <v>6.3049804076999996</v>
-      </c>
-      <c r="G42">
-        <v>15.478</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.459</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1407,22 +1277,19 @@
         <v>4.05</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>-2.0710000000000002</v>
       </c>
       <c r="D43">
-        <v>1.9410000000000001</v>
+        <v>15.61</v>
       </c>
       <c r="E43">
-        <v>19.731356300000002</v>
+        <v>2.0739999999999998</v>
       </c>
       <c r="F43">
-        <v>6.6096794280999998</v>
-      </c>
-      <c r="G43">
-        <v>15.324999999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.201000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1430,22 +1297,19 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>-2.0579999999999998</v>
       </c>
       <c r="D44">
-        <v>2.0019999999999998</v>
+        <v>15.718</v>
       </c>
       <c r="E44">
-        <v>19.865046869999997</v>
+        <v>2.0910000000000002</v>
       </c>
       <c r="F44">
-        <v>6.5477726134999994</v>
-      </c>
-      <c r="G44">
-        <v>15.103999999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.929</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1453,22 +1317,19 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>-2.0710000000000002</v>
       </c>
       <c r="D45">
-        <v>1.9650000000000001</v>
+        <v>15.831</v>
       </c>
       <c r="E45">
-        <v>19.961497700000002</v>
+        <v>2.1989999999999998</v>
       </c>
       <c r="F45">
-        <v>6.4422721251999997</v>
-      </c>
-      <c r="G45">
-        <v>14.919999999999998</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.804</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1476,22 +1337,19 @@
         <v>4.2</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>-2.0990000000000002</v>
       </c>
       <c r="D46">
-        <v>1.9570000000000001</v>
+        <v>15.949</v>
       </c>
       <c r="E46">
-        <v>20.281917499999999</v>
+        <v>2.1989999999999998</v>
       </c>
       <c r="F46">
-        <v>6.7648320769999994</v>
-      </c>
-      <c r="G46">
-        <v>14.89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.603</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1499,22 +1357,19 @@
         <v>4.25</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>-2.0960000000000001</v>
       </c>
       <c r="D47">
-        <v>1.9850000000000001</v>
+        <v>16.058</v>
       </c>
       <c r="E47">
-        <v>20.137319529999999</v>
+        <v>2.1659999999999999</v>
       </c>
       <c r="F47">
-        <v>6.5474223937999998</v>
-      </c>
-      <c r="G47">
-        <v>14.7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.468</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1522,22 +1377,19 @@
         <v>4.3</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>-2.0880000000000001</v>
       </c>
       <c r="D48">
-        <v>1.9930000000000001</v>
+        <v>16.151</v>
       </c>
       <c r="E48">
-        <v>20.362427400000001</v>
+        <v>2.2570000000000001</v>
       </c>
       <c r="F48">
-        <v>6.6657602691999998</v>
-      </c>
-      <c r="G48">
-        <v>14.763999999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.532999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1545,22 +1397,19 @@
         <v>4.3499999999999996</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>-2.1120000000000001</v>
       </c>
       <c r="D49">
-        <v>1.98</v>
+        <v>16.212</v>
       </c>
       <c r="E49">
-        <v>20.448902</v>
+        <v>2.2149999999999999</v>
       </c>
       <c r="F49">
-        <v>6.7482532959000006</v>
-      </c>
-      <c r="G49">
-        <v>14.824</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.544</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1568,22 +1417,19 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>-2.1160000000000001</v>
       </c>
       <c r="D50">
-        <v>1.996</v>
+        <v>16.238</v>
       </c>
       <c r="E50">
-        <v>20.482333199999999</v>
+        <v>2.198</v>
       </c>
       <c r="F50">
-        <v>6.7257624206999997</v>
-      </c>
-      <c r="G50">
-        <v>14.933</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.670999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1591,22 +1437,19 @@
         <v>4.45</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>-2.1469999999999998</v>
       </c>
       <c r="D51">
-        <v>2.0270000000000001</v>
+        <v>16.225999999999999</v>
       </c>
       <c r="E51">
-        <v>20.420257929999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F51">
-        <v>6.6785746002000002</v>
-      </c>
-      <c r="G51">
-        <v>15.167</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.882999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1614,22 +1457,19 @@
         <v>4.5</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>-2.1539999999999999</v>
       </c>
       <c r="D52">
-        <v>2.0219999999999998</v>
+        <v>16.184000000000001</v>
       </c>
       <c r="E52">
-        <v>20.488780599999998</v>
+        <v>2.2050000000000001</v>
       </c>
       <c r="F52">
-        <v>6.7511266174000006</v>
-      </c>
-      <c r="G52">
-        <v>15.418000000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1637,22 +1477,19 @@
         <v>4.55</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>-2.1920000000000002</v>
       </c>
       <c r="D53">
-        <v>2.0289999999999999</v>
+        <v>16.106000000000002</v>
       </c>
       <c r="E53">
-        <v>20.3821105</v>
+        <v>2.2029999999999998</v>
       </c>
       <c r="F53">
-        <v>6.6168840941999996</v>
-      </c>
-      <c r="G53">
-        <v>15.600000000000001</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.343999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1660,22 +1497,19 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>-2.161</v>
       </c>
       <c r="D54">
-        <v>2.1</v>
+        <v>16.007999999999999</v>
       </c>
       <c r="E54">
-        <v>20.315310969999999</v>
+        <v>2.1739999999999999</v>
       </c>
       <c r="F54">
-        <v>6.6606535796999999</v>
-      </c>
-      <c r="G54">
-        <v>15.759</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.472</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1683,22 +1517,19 @@
         <v>4.6500000000000004</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>-2.1629999999999998</v>
       </c>
       <c r="D55">
-        <v>2.0230000000000001</v>
+        <v>15.896000000000001</v>
       </c>
       <c r="E55">
-        <v>20.278176999999999</v>
+        <v>2.1890000000000001</v>
       </c>
       <c r="F55">
-        <v>6.8535843048000009</v>
-      </c>
-      <c r="G55">
-        <v>15.914000000000001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.555</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1706,22 +1537,19 @@
         <v>4.7</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>-2.2679999999999998</v>
       </c>
       <c r="D56">
-        <v>2.089</v>
+        <v>15.784000000000001</v>
       </c>
       <c r="E56">
-        <v>20.165608499999998</v>
+        <v>2.1779999999999999</v>
       </c>
       <c r="F56">
-        <v>6.8903919983000002</v>
-      </c>
-      <c r="G56">
-        <v>15.907</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.504</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1729,22 +1557,19 @@
         <v>4.75</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>-2.2429999999999999</v>
       </c>
       <c r="D57">
-        <v>2.169</v>
+        <v>15.682</v>
       </c>
       <c r="E57">
-        <v>20.154103709999998</v>
+        <v>2.2909999999999999</v>
       </c>
       <c r="F57">
-        <v>6.9753902283000002</v>
-      </c>
-      <c r="G57">
-        <v>15.872</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.465999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1752,22 +1577,19 @@
         <v>4.8</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>-2.169</v>
       </c>
       <c r="D58">
-        <v>2.1019999999999999</v>
+        <v>15.587</v>
       </c>
       <c r="E58">
-        <v>19.960003629999999</v>
+        <v>2.2240000000000002</v>
       </c>
       <c r="F58">
-        <v>6.9093153991999996</v>
-      </c>
-      <c r="G58">
-        <v>15.657999999999999</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.195</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1775,22 +1597,19 @@
         <v>4.8499999999999996</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>-2.2959999999999998</v>
       </c>
       <c r="D59">
-        <v>2.0830000000000002</v>
+        <v>15.512</v>
       </c>
       <c r="E59">
-        <v>19.890742699999997</v>
+        <v>2.2069999999999999</v>
       </c>
       <c r="F59">
-        <v>6.8571367493000004</v>
-      </c>
-      <c r="G59">
-        <v>15.394</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.919</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1798,22 +1617,19 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>-2.2519999999999998</v>
       </c>
       <c r="D60">
-        <v>2.2010000000000001</v>
+        <v>15.46</v>
       </c>
       <c r="E60">
-        <v>20.013492500000002</v>
+        <v>2.343</v>
       </c>
       <c r="F60">
-        <v>7.188580108600001</v>
-      </c>
-      <c r="G60">
-        <v>15.361000000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.821999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1821,22 +1637,19 @@
         <v>4.95</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>-2.2650000000000001</v>
       </c>
       <c r="D61">
-        <v>2.1360000000000001</v>
+        <v>15.423999999999999</v>
       </c>
       <c r="E61">
-        <v>19.813616969999998</v>
+        <v>2.3519999999999999</v>
       </c>
       <c r="F61">
-        <v>7.0670668335000002</v>
-      </c>
-      <c r="G61">
-        <v>15.141000000000002</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.624000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1844,19 +1657,416 @@
         <v>5</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>-2.2650000000000001</v>
       </c>
       <c r="D62">
-        <v>2.1549999999999998</v>
+        <v>15.425000000000001</v>
       </c>
       <c r="E62">
-        <v>19.9721045</v>
+        <v>2.37</v>
       </c>
       <c r="F62">
-        <v>7.2718139342999999</v>
-      </c>
-      <c r="G62">
-        <v>15.097000000000001</v>
+        <v>10.513</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>5.05</v>
+      </c>
+      <c r="C63">
+        <v>-2.3180000000000001</v>
+      </c>
+      <c r="D63">
+        <v>15.445</v>
+      </c>
+      <c r="E63">
+        <v>2.415</v>
+      </c>
+      <c r="F63">
+        <v>10.505000000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C64">
+        <v>-2.319</v>
+      </c>
+      <c r="D64">
+        <v>15.497</v>
+      </c>
+      <c r="E64">
+        <v>2.4409999999999998</v>
+      </c>
+      <c r="F64">
+        <v>10.573</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>5.15</v>
+      </c>
+      <c r="C65">
+        <v>-2.359</v>
+      </c>
+      <c r="D65">
+        <v>15.574999999999999</v>
+      </c>
+      <c r="E65">
+        <v>2.4319999999999999</v>
+      </c>
+      <c r="F65">
+        <v>10.68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>5.2</v>
+      </c>
+      <c r="C66">
+        <v>-2.3319999999999999</v>
+      </c>
+      <c r="D66">
+        <v>15.673</v>
+      </c>
+      <c r="E66">
+        <v>2.4319999999999999</v>
+      </c>
+      <c r="F66">
+        <v>10.881</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>5.25</v>
+      </c>
+      <c r="C67">
+        <v>-2.3340000000000001</v>
+      </c>
+      <c r="D67">
+        <v>15.789</v>
+      </c>
+      <c r="E67">
+        <v>2.4129999999999998</v>
+      </c>
+      <c r="F67">
+        <v>11.102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>5.3</v>
+      </c>
+      <c r="C68">
+        <v>-2.3650000000000002</v>
+      </c>
+      <c r="D68">
+        <v>15.901</v>
+      </c>
+      <c r="E68">
+        <v>2.3620000000000001</v>
+      </c>
+      <c r="F68">
+        <v>11.29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>5.35</v>
+      </c>
+      <c r="C69">
+        <v>-2.371</v>
+      </c>
+      <c r="D69">
+        <v>16.012</v>
+      </c>
+      <c r="E69">
+        <v>2.4129999999999998</v>
+      </c>
+      <c r="F69">
+        <v>11.574</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>5.4</v>
+      </c>
+      <c r="C70">
+        <v>-2.3780000000000001</v>
+      </c>
+      <c r="D70">
+        <v>16.109000000000002</v>
+      </c>
+      <c r="E70">
+        <v>2.4129999999999998</v>
+      </c>
+      <c r="F70">
+        <v>11.696999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>5.45</v>
+      </c>
+      <c r="C71">
+        <v>-2.3759999999999999</v>
+      </c>
+      <c r="D71">
+        <v>16.184999999999999</v>
+      </c>
+      <c r="E71">
+        <v>2.387</v>
+      </c>
+      <c r="F71">
+        <v>11.728999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>5.5</v>
+      </c>
+      <c r="C72">
+        <v>-2.4209999999999998</v>
+      </c>
+      <c r="D72">
+        <v>16.224</v>
+      </c>
+      <c r="E72">
+        <v>2.411</v>
+      </c>
+      <c r="F72">
+        <v>11.672000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>5.55</v>
+      </c>
+      <c r="C73">
+        <v>-2.395</v>
+      </c>
+      <c r="D73">
+        <v>16.239000000000001</v>
+      </c>
+      <c r="E73">
+        <v>2.4740000000000002</v>
+      </c>
+      <c r="F73">
+        <v>11.566000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>5.6</v>
+      </c>
+      <c r="C74">
+        <v>-2.4470000000000001</v>
+      </c>
+      <c r="D74">
+        <v>16.222000000000001</v>
+      </c>
+      <c r="E74">
+        <v>2.484</v>
+      </c>
+      <c r="F74">
+        <v>11.347</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>5.65</v>
+      </c>
+      <c r="C75">
+        <v>-2.4620000000000002</v>
+      </c>
+      <c r="D75">
+        <v>16.175999999999998</v>
+      </c>
+      <c r="E75">
+        <v>2.4769999999999999</v>
+      </c>
+      <c r="F75">
+        <v>11.09</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>5.7</v>
+      </c>
+      <c r="C76">
+        <v>-2.4279999999999999</v>
+      </c>
+      <c r="D76">
+        <v>16.109000000000002</v>
+      </c>
+      <c r="E76">
+        <v>2.524</v>
+      </c>
+      <c r="F76">
+        <v>10.911</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>5.75</v>
+      </c>
+      <c r="C77">
+        <v>-2.4159999999999999</v>
+      </c>
+      <c r="D77">
+        <v>16.021999999999998</v>
+      </c>
+      <c r="E77">
+        <v>2.5590000000000002</v>
+      </c>
+      <c r="F77">
+        <v>10.78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>5.8</v>
+      </c>
+      <c r="C78">
+        <v>-2.5179999999999998</v>
+      </c>
+      <c r="D78">
+        <v>15.914</v>
+      </c>
+      <c r="E78">
+        <v>2.556</v>
+      </c>
+      <c r="F78">
+        <v>10.683999999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>5.85</v>
+      </c>
+      <c r="C79">
+        <v>-2.4830000000000001</v>
+      </c>
+      <c r="D79">
+        <v>15.805</v>
+      </c>
+      <c r="E79">
+        <v>2.5720000000000001</v>
+      </c>
+      <c r="F79">
+        <v>10.696999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>5.9</v>
+      </c>
+      <c r="C80">
+        <v>-2.452</v>
+      </c>
+      <c r="D80">
+        <v>15.693</v>
+      </c>
+      <c r="E80">
+        <v>2.5619999999999998</v>
+      </c>
+      <c r="F80">
+        <v>10.772</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>5.95</v>
+      </c>
+      <c r="C81">
+        <v>-2.5230000000000001</v>
+      </c>
+      <c r="D81">
+        <v>15.590999999999999</v>
+      </c>
+      <c r="E81">
+        <v>2.5710000000000002</v>
+      </c>
+      <c r="F81">
+        <v>10.939</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>6</v>
+      </c>
+      <c r="C82">
+        <v>-2.528</v>
+      </c>
+      <c r="D82">
+        <v>15.506</v>
+      </c>
+      <c r="E82">
+        <v>2.5870000000000002</v>
+      </c>
+      <c r="F82">
+        <v>11.170999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>